<commit_message>
fixed utilisations and costs
</commit_message>
<xml_diff>
--- a/data-raw/8d_cost_utilisation_intervention.xlsx
+++ b/data-raw/8d_cost_utilisation_intervention.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/cea-glaucoma-ai-screening/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0942171-43F1-4C45-B743-F64F41D2840E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F12AF47-FC1F-7F46-873B-ACB046D5BA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31500" yWindow="1380" windowWidth="34400" windowHeight="28300" xr2:uid="{C3F4995C-3B70-6C49-A03D-B152E04542DC}"/>
+    <workbookView xWindow="31500" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{C3F4995C-3B70-6C49-A03D-B152E04542DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,36 +74,9 @@
     <t>price</t>
   </si>
   <si>
-    <t>surgery_5</t>
-  </si>
-  <si>
     <t>TCP</t>
   </si>
   <si>
-    <t>laser_1</t>
-  </si>
-  <si>
-    <t>laser_2</t>
-  </si>
-  <si>
-    <t>laser_3</t>
-  </si>
-  <si>
-    <t>laser_4</t>
-  </si>
-  <si>
-    <t>surgery_1</t>
-  </si>
-  <si>
-    <t>surgery_2</t>
-  </si>
-  <si>
-    <t>surgery_3</t>
-  </si>
-  <si>
-    <t>surgery_4</t>
-  </si>
-  <si>
     <t>laser_mild</t>
   </si>
   <si>
@@ -126,6 +99,33 @@
   </si>
   <si>
     <t>surgery_vi</t>
+  </si>
+  <si>
+    <t>laser_treatment_1</t>
+  </si>
+  <si>
+    <t>laser_treatment_2</t>
+  </si>
+  <si>
+    <t>laser_treatment_3</t>
+  </si>
+  <si>
+    <t>laser_treatment_4</t>
+  </si>
+  <si>
+    <t>surgery_treatment_1</t>
+  </si>
+  <si>
+    <t>surgery_treatment_2</t>
+  </si>
+  <si>
+    <t>surgery_treatment_3</t>
+  </si>
+  <si>
+    <t>surgery_treatment_4</t>
+  </si>
+  <si>
+    <t>surgery_treatment_5</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -599,7 +599,7 @@
     </row>
     <row r="2" spans="1:4" ht="70" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -612,8 +612,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="53" thickTop="1" thickBot="1">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
+      <c r="A3" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -626,8 +626,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="87" thickTop="1" thickBot="1">
-      <c r="A4" s="4" t="s">
-        <v>16</v>
+      <c r="A4" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -640,8 +640,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="121" thickTop="1" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
+      <c r="A5" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="6" spans="1:4" ht="53" thickTop="1" thickBot="1">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -668,8 +668,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="70" thickTop="1" thickBot="1">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
+      <c r="A7" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="8" spans="1:4" ht="70" thickTop="1" thickBot="1">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -696,8 +696,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="87" thickTop="1" thickBot="1">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
+      <c r="A9" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -709,12 +709,12 @@
         <v>474.66</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="19" thickTop="1" thickBot="1">
+    <row r="10" spans="1:4" ht="36" thickTop="1" thickBot="1">
       <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>4.1000000000000002E-2</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="11" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>0.51</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="12" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1">
         <v>0.21999999999999997</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="13" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
         <v>0.18</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="14" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
         <v>0.11000000000000001</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="15" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
         <v>4.3999999999999997E-2</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="16" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1">
         <v>0.28599999999999998</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="17" spans="1:3" ht="18" thickTop="1" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1">
         <v>0.45</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="18" spans="1:3" ht="18" thickTop="1" thickBot="1">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1">
         <v>0.22000000000000003</v>

</xml_diff>

<commit_message>
model validation and small bug fixes
</commit_message>
<xml_diff>
--- a/data-raw/8d_cost_utilisation_intervention.xlsx
+++ b/data-raw/8d_cost_utilisation_intervention.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart-janb/Documents/GitHub/cea-glaucoma-ai-screening/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBDD38B-B1CE-9C4B-B4E2-59B5CBED9E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45B5BC6-C3BF-A44D-9FDD-6486D69AEA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41780" yWindow="800" windowWidth="34400" windowHeight="21100" xr2:uid="{C3F4995C-3B70-6C49-A03D-B152E04542DC}"/>
+    <workbookView xWindow="41900" yWindow="500" windowWidth="34400" windowHeight="21100" xr2:uid="{C3F4995C-3B70-6C49-A03D-B152E04542DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E20757A-CBE6-1F41-85A5-572B7D012FB2}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -620,7 +620,7 @@
         <v>0.16</v>
       </c>
       <c r="F2" s="8">
-        <v>155.94</v>
+        <v>858.82</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="53" thickTop="1" thickBot="1">
@@ -640,7 +640,7 @@
         <v>0.47500000000000003</v>
       </c>
       <c r="F3" s="8">
-        <v>406.66999999999996</v>
+        <v>378.83</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="87" thickTop="1" thickBot="1">
@@ -660,7 +660,7 @@
         <v>4.2200000000000001E-2</v>
       </c>
       <c r="F4" s="8">
-        <v>155.94</v>
+        <v>128.1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="121" thickTop="1" thickBot="1">
@@ -700,7 +700,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="F6" s="8">
-        <v>474.66</v>
+        <v>751.9</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="70" thickTop="1" thickBot="1">
@@ -720,7 +720,7 @@
         <v>1.4300000000000002E-2</v>
       </c>
       <c r="F7" s="8">
-        <v>474.66</v>
+        <v>751.9</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="70" thickTop="1" thickBot="1">
@@ -740,7 +740,7 @@
         <v>2.5500000000000002E-2</v>
       </c>
       <c r="F8" s="8">
-        <v>474.66</v>
+        <v>751.9</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="87" thickTop="1" thickBot="1">
@@ -760,7 +760,7 @@
         <v>0.16799999999999998</v>
       </c>
       <c r="F9" s="8">
-        <v>474.66</v>
+        <v>1938.76</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" thickTop="1" thickBot="1">

</xml_diff>